<commit_message>
changes to previous assignments
</commit_message>
<xml_diff>
--- a/01-Exploring_Plotting_Excel/ProductionPivot_Complete (Assignment_1).xlsx
+++ b/01-Exploring_Plotting_Excel/ProductionPivot_Complete (Assignment_1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Books\Netflix Bootcamp\Netflix Assignments\01-Exploring_Plotting_Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\NFLX-VIRT-DATA-PT-08-2021-E-LOL\02-Assignments\01-Introduction\01-Exploring_Plotting_Excel\Unsolved\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD854444-A0E1-4603-88C4-8BC958CCEAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D5D54B-E0D9-49BF-9079-23F91BA3A00F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="2" r:id="rId1"/>
@@ -22,10 +22,22 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Orders!$H$1</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Orders!$H$2:$H$601</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Orders!$H$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Orders!$H$2:$H$601</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Orders!$H$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Orders!$H$2:$H$601</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Orders!$A$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Orders!$A$2:$A$601</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Orders!$H$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Orders!$H$2:$H$601</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Orders!$A$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Orders!$A$2:$A$601</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Orders!$H$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Orders!$H$2:$H$601</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="7" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -45,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="34">
   <si>
     <t>Product Name</t>
   </si>
@@ -322,7 +334,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[ProductionPivot_Complete (Assignment_1).xlsx]Pivot Table 2 (Q4)!PivotTable2</c:name>
+    <c:name>[ProductionPivot_Unsolved.xlsx]Pivot Table 2 (Q4)!PivotTable2</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -636,246 +648,6 @@
           <a:effectLst/>
         </c:spPr>
       </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="17"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="FFC000"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="18"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="FFC000"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="19"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="FFC000"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="20"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="FFC000"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="21"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="7030A0"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="22"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="7030A0"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="23"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="7030A0"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="24"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="7030A0"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="25"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="002060"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="26"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="002060"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="27"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="002060"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="28"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="002060"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="29"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="92D050"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="30"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="92D050"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="31"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="92D050"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="32"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="92D050"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="33"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="00B0F0"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="34"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="00B0F0"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="35"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="00B0F0"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="36"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="00B0F0"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -913,7 +685,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FFC000"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -932,7 +704,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FFC000"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -951,7 +723,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FFC000"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -970,7 +742,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FFC000"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -989,7 +761,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:srgbClr val="FFFF00"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1008,7 +780,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:srgbClr val="FFFF00"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1027,7 +799,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:srgbClr val="FFFF00"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1046,7 +818,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:srgbClr val="FFFF00"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1065,7 +837,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="7030A0"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1084,7 +856,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="7030A0"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1103,7 +875,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="7030A0"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1122,7 +894,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="7030A0"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1139,6 +911,15 @@
             <c:idx val="12"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000F-D037-41E9-A645-7BC3D5408989}"/>
@@ -1147,376 +928,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000010-D037-41E9-A645-7BC3D5408989}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="14"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000011-D037-41E9-A645-7BC3D5408989}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="15"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000012-D037-41E9-A645-7BC3D5408989}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="16"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="17"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="18"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="19"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="20"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000021-2CA3-4E71-949A-4B81ECF67F2A}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="21"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000022-2CA3-4E71-949A-4B81ECF67F2A}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="22"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000023-2CA3-4E71-949A-4B81ECF67F2A}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="23"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000024-2CA3-4E71-949A-4B81ECF67F2A}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="24"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="92D050"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000025-2CA3-4E71-949A-4B81ECF67F2A}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="25"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="92D050"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000026-2CA3-4E71-949A-4B81ECF67F2A}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="26"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="92D050"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000027-2CA3-4E71-949A-4B81ECF67F2A}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="27"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="92D050"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000028-2CA3-4E71-949A-4B81ECF67F2A}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="28"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000029-2CA3-4E71-949A-4B81ECF67F2A}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="29"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000002A-2CA3-4E71-949A-4B81ECF67F2A}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="30"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000002B-2CA3-4E71-949A-4B81ECF67F2A}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="31"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000002C-2CA3-4E71-949A-4B81ECF67F2A}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="32"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="33"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="34"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="35"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="60"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1528,9 +939,14 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000010-D037-41E9-A645-7BC3D5408989}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="61"/>
+            <c:idx val="14"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1542,9 +958,14 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-D037-41E9-A645-7BC3D5408989}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="62"/>
+            <c:idx val="15"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1556,26 +977,17 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="63"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="0070C0"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000012-D037-41E9-A645-7BC3D5408989}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Pivot Table 2 (Q4)'!$A$4:$A$89</c:f>
+              <c:f>'Pivot Table 2 (Q4)'!$A$4:$A$24</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="68"/>
+                <c:ptCount val="16"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>High</c:v>
@@ -1625,214 +1037,19 @@
                   <c:pt idx="15">
                     <c:v>VIP</c:v>
                   </c:pt>
-                  <c:pt idx="16">
-                    <c:v>High</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>Low</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>Medium</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>VIP</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>High</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>Low</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>Medium</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>VIP</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>High</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>Low</c:v>
-                  </c:pt>
-                  <c:pt idx="26">
-                    <c:v>Medium</c:v>
-                  </c:pt>
-                  <c:pt idx="27">
-                    <c:v>VIP</c:v>
-                  </c:pt>
-                  <c:pt idx="28">
-                    <c:v>High</c:v>
-                  </c:pt>
-                  <c:pt idx="29">
-                    <c:v>Low</c:v>
-                  </c:pt>
-                  <c:pt idx="30">
-                    <c:v>Medium</c:v>
-                  </c:pt>
-                  <c:pt idx="31">
-                    <c:v>VIP</c:v>
-                  </c:pt>
-                  <c:pt idx="32">
-                    <c:v>High</c:v>
-                  </c:pt>
-                  <c:pt idx="33">
-                    <c:v>Low</c:v>
-                  </c:pt>
-                  <c:pt idx="34">
-                    <c:v>Medium</c:v>
-                  </c:pt>
-                  <c:pt idx="35">
-                    <c:v>VIP</c:v>
-                  </c:pt>
-                  <c:pt idx="36">
-                    <c:v>High</c:v>
-                  </c:pt>
-                  <c:pt idx="37">
-                    <c:v>Low</c:v>
-                  </c:pt>
-                  <c:pt idx="38">
-                    <c:v>Medium</c:v>
-                  </c:pt>
-                  <c:pt idx="39">
-                    <c:v>VIP</c:v>
-                  </c:pt>
-                  <c:pt idx="40">
-                    <c:v>High</c:v>
-                  </c:pt>
-                  <c:pt idx="41">
-                    <c:v>Low</c:v>
-                  </c:pt>
-                  <c:pt idx="42">
-                    <c:v>Medium</c:v>
-                  </c:pt>
-                  <c:pt idx="43">
-                    <c:v>VIP</c:v>
-                  </c:pt>
-                  <c:pt idx="44">
-                    <c:v>High</c:v>
-                  </c:pt>
-                  <c:pt idx="45">
-                    <c:v>Low</c:v>
-                  </c:pt>
-                  <c:pt idx="46">
-                    <c:v>Medium</c:v>
-                  </c:pt>
-                  <c:pt idx="47">
-                    <c:v>VIP</c:v>
-                  </c:pt>
-                  <c:pt idx="48">
-                    <c:v>High</c:v>
-                  </c:pt>
-                  <c:pt idx="49">
-                    <c:v>Low</c:v>
-                  </c:pt>
-                  <c:pt idx="50">
-                    <c:v>Medium</c:v>
-                  </c:pt>
-                  <c:pt idx="51">
-                    <c:v>VIP</c:v>
-                  </c:pt>
-                  <c:pt idx="52">
-                    <c:v>High</c:v>
-                  </c:pt>
-                  <c:pt idx="53">
-                    <c:v>Low</c:v>
-                  </c:pt>
-                  <c:pt idx="54">
-                    <c:v>Medium</c:v>
-                  </c:pt>
-                  <c:pt idx="55">
-                    <c:v>VIP</c:v>
-                  </c:pt>
-                  <c:pt idx="56">
-                    <c:v>High</c:v>
-                  </c:pt>
-                  <c:pt idx="57">
-                    <c:v>Low</c:v>
-                  </c:pt>
-                  <c:pt idx="58">
-                    <c:v>Medium</c:v>
-                  </c:pt>
-                  <c:pt idx="59">
-                    <c:v>VIP</c:v>
-                  </c:pt>
-                  <c:pt idx="60">
-                    <c:v>High</c:v>
-                  </c:pt>
-                  <c:pt idx="61">
-                    <c:v>Low</c:v>
-                  </c:pt>
-                  <c:pt idx="62">
-                    <c:v>Medium</c:v>
-                  </c:pt>
-                  <c:pt idx="63">
-                    <c:v>VIP</c:v>
-                  </c:pt>
-                  <c:pt idx="64">
-                    <c:v>High</c:v>
-                  </c:pt>
-                  <c:pt idx="65">
-                    <c:v>Low</c:v>
-                  </c:pt>
-                  <c:pt idx="66">
-                    <c:v>Medium</c:v>
-                  </c:pt>
-                  <c:pt idx="67">
-                    <c:v>VIP</c:v>
-                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>10 Foot HDMI Cable</c:v>
+                    <c:v>10 Foot USB Cable</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>10 Foot USB Cable</c:v>
+                    <c:v>2 Foot USB Cable</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>128GB Flash Drive</c:v>
+                    <c:v>64GB Flash Drive</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>16GB Flash Drive</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>2 Foot USB Cable</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>32GB Flash Drive</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>5 Foot HDMI Cable</c:v>
-                  </c:pt>
-                  <c:pt idx="28">
-                    <c:v>5 Foot USB Cable</c:v>
-                  </c:pt>
-                  <c:pt idx="32">
-                    <c:v>64GB Flash Drive</c:v>
-                  </c:pt>
-                  <c:pt idx="36">
-                    <c:v>Blue Ray DVD</c:v>
-                  </c:pt>
-                  <c:pt idx="40">
-                    <c:v>Bluetooth Keyboard</c:v>
-                  </c:pt>
-                  <c:pt idx="44">
-                    <c:v>Bluetooth Mouse</c:v>
-                  </c:pt>
-                  <c:pt idx="48">
-                    <c:v>Standard Edition DVD</c:v>
-                  </c:pt>
-                  <c:pt idx="52">
-                    <c:v>VHS Tape</c:v>
-                  </c:pt>
-                  <c:pt idx="56">
-                    <c:v>Wired Keyboard</c:v>
-                  </c:pt>
-                  <c:pt idx="60">
                     <c:v>Wired Mouse</c:v>
-                  </c:pt>
-                  <c:pt idx="64">
-                    <c:v>Wireless Router</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -1840,213 +1057,57 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pivot Table 2 (Q4)'!$B$4:$B$89</c:f>
+              <c:f>'Pivot Table 2 (Q4)'!$B$4:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="11">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>6</c:v>
-                </c:pt>
                 <c:pt idx="15">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="20">
                   <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2304,45 +1365,42 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
     <cx:title pos="t" align="ctr" overlay="0">
       <cx:tx>
-        <cx:txData>
-          <cx:v>Totals distribution </cx:v>
-        </cx:txData>
+        <cx:rich>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              </a:rPr>
+              <a:t>Totals distribution </a:t>
+            </a:r>
+          </a:p>
+        </cx:rich>
       </cx:tx>
-      <cx:txPr>
-        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr" rtl="0">
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:sysClr>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-            </a:rPr>
-            <a:t>Totals distribution </a:t>
-          </a:r>
-        </a:p>
-      </cx:txPr>
     </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
         <cx:series layoutId="clusteredColumn" uniqueId="{E0602BB1-C8A6-4937-818D-8253B201D2ED}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:f>_xlchart.v1.10</cx:f>
               <cx:v>Total</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3466,16 +2524,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>361949</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>23810</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>52385</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>600074</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10262,7 +9320,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A6A1F0A3-EFAB-4FA5-A6F4-7FF16B5F5C6B}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A6A1F0A3-EFAB-4FA5-A6F4-7FF16B5F5C6B}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -10337,7 +9395,7 @@
     </format>
   </formats>
   <conditionalFormats count="2">
-    <conditionalFormat priority="1">
+    <conditionalFormat priority="2">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="2">
@@ -10356,7 +9414,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="2">
+    <conditionalFormat priority="1">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="2">
@@ -10389,8 +9447,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F90466E5-BCE4-4761-84FD-B38EAF0DF251}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:B89" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F90466E5-BCE4-4761-84FD-B38EAF0DF251}" name="PivotTable2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:B24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0">
@@ -10999,7 +10057,7 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisRow" showAll="0" measureFilter="1">
       <items count="18">
         <item x="4"/>
         <item x="0"/>
@@ -11038,54 +10096,9 @@
     <field x="3"/>
     <field x="4"/>
   </rowFields>
-  <rowItems count="86">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
+  <rowItems count="21">
     <i>
       <x v="1"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="3"/>
     </i>
     <i r="1">
       <x/>
@@ -11115,142 +10128,7 @@
       <x v="3"/>
     </i>
     <i>
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
       <x v="8"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="14"/>
     </i>
     <i r="1">
       <x/>
@@ -11279,21 +10157,6 @@
     <i r="1">
       <x v="3"/>
     </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
     <i t="grand">
       <x/>
     </i>
@@ -11304,7 +10167,7 @@
   <dataFields count="1">
     <dataField name="Count of Order Number" fld="1" subtotal="count" baseField="3" baseItem="0"/>
   </dataFields>
-  <chartFormats count="37">
+  <chartFormats count="17">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -11554,308 +10417,19 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="17">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="18">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="19">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="20">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="21">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="22">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="23">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="24">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="25">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="26">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="27">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="28">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="29">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="30">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="31">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="32">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="33">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="34">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="35">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="36">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <filters count="1">
+    <filter fld="3" type="valueGreaterThan" evalOrder="-1" id="2" iMeasureFld="0">
+      <autoFilter ref="A1">
+        <filterColumn colId="0">
+          <customFilters>
+            <customFilter operator="greaterThan" val="40"/>
+          </customFilters>
+        </filterColumn>
+      </autoFilter>
+    </filter>
+  </filters>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
@@ -11868,7 +10442,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{10271174-3EAF-43C6-8CAA-3AB585BE7710}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{10271174-3EAF-43C6-8CAA-3AB585BE7710}" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -28569,15 +27143,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44589FEB-CBA9-47AB-9197-0F2E40CABA4A}">
-  <dimension ref="A3:B89"/>
+  <dimension ref="A3:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -28591,10 +27165,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" s="4">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -28602,7 +27176,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="4">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -28610,7 +27184,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="4">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -28618,7 +27192,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="4">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -28626,12 +27200,12 @@
         <v>22</v>
       </c>
       <c r="B8" s="4">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B9" s="4">
         <v>46</v>
@@ -28642,7 +27216,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="4">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -28650,7 +27224,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="4">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -28658,7 +27232,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="4">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -28666,15 +27240,15 @@
         <v>22</v>
       </c>
       <c r="B13" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="4">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -28682,7 +27256,7 @@
         <v>21</v>
       </c>
       <c r="B15" s="4">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -28690,7 +27264,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="4">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -28698,7 +27272,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="4">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -28706,15 +27280,15 @@
         <v>22</v>
       </c>
       <c r="B18" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B19" s="4">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -28722,7 +27296,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="4">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -28730,7 +27304,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="4">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -28738,7 +27312,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="4">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -28746,535 +27320,15 @@
         <v>22</v>
       </c>
       <c r="B23" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B24" s="4">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="4">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" s="4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B37" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B39" s="4">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B40" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="4">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B42" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B43" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B44" s="4">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B46" s="4">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B47" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B48" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B49" s="4">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B50" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B51" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B52" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B53" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B54" s="4">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B55" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B56" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B57" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B58" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B59" s="4">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B60" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B61" s="4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B62" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B63" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B64" s="4">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B65" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B66" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B67" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B68" s="4">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B69" s="4">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B70" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B71" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B72" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B73" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B74" s="4">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B75" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B76" s="4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B77" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B78" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B79" s="4">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B80" s="4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B81" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B82" s="4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B83" s="4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B84" s="4">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B85" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B86" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B87" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B88" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B89" s="4">
-        <v>600</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -29370,7 +27424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4CAFA7-D6DE-4B6B-A682-B443202F3AEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>

</xml_diff>